<commit_message>
wp. move to json data master. all tests passing, however cli needs testing
</commit_message>
<xml_diff>
--- a/tests/resources/250_master_test_1.xlsx
+++ b/tests/resources/250_master_test_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="289">
   <si>
     <t xml:space="preserve">PROJECT ID</t>
   </si>
@@ -409,7 +409,7 @@
     <t xml:space="preserve">MM20 Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">R1 name</t>
+    <t xml:space="preserve">R1 name </t>
   </si>
   <si>
     <t xml:space="preserve">R1 needed by</t>
@@ -421,49 +421,73 @@
     <t xml:space="preserve">R1 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R1 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R1 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R2 name</t>
+    <t xml:space="preserve">R2 name </t>
   </si>
   <si>
     <t xml:space="preserve">R2 needed by</t>
   </si>
   <si>
-    <t xml:space="preserve">R2 escalated to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2 type</t>
+    <t xml:space="preserve">R2 escalated to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 Point of Contact</t>
   </si>
   <si>
     <t xml:space="preserve">R2 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R3 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3 escalated to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3 type</t>
+    <t xml:space="preserve">R3 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 escalated to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 Point of Contact</t>
   </si>
   <si>
     <t xml:space="preserve">R3 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R4 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4 escalated to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4 type</t>
+    <t xml:space="preserve">R4 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4 escalated to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4 type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4 Point of Contact</t>
   </si>
   <si>
     <t xml:space="preserve">R4 secured</t>
@@ -472,97 +496,133 @@
     <t xml:space="preserve">R5 name</t>
   </si>
   <si>
-    <t xml:space="preserve">R5 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5 escalated to</t>
+    <t xml:space="preserve">R5 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R5 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R5 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R5 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R6 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6 escalated to</t>
+    <t xml:space="preserve">R6 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R6 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R6 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R6 secured</t>
   </si>
   <si>
     <t xml:space="preserve">R7 name</t>
   </si>
   <si>
-    <t xml:space="preserve">R7 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7 escalated to</t>
+    <t xml:space="preserve">R7 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R7 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R7 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R7 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R8 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8 escalated to</t>
+    <t xml:space="preserve">R8 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R8 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R8 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R8 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R9 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9 escalated to</t>
+    <t xml:space="preserve">R9 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R9 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R9 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R9 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R10 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10 escalated to</t>
+    <t xml:space="preserve">R10 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R10 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R10 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R10 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R11 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11 needed by</t>
+    <t xml:space="preserve">R11 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11 needed by </t>
   </si>
   <si>
     <t xml:space="preserve">R11 escalated to</t>
@@ -571,28 +631,40 @@
     <t xml:space="preserve">R11 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R11 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R11 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R12 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12 escalated to</t>
+    <t xml:space="preserve">R12 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R12 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R12 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R12 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R13 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R13 needed by</t>
+    <t xml:space="preserve">R13 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13 needed by </t>
   </si>
   <si>
     <t xml:space="preserve">R13 escalated to</t>
@@ -601,25 +673,37 @@
     <t xml:space="preserve">R13 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R13 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R13 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R14 name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14 needed by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14 escalated to</t>
+    <t xml:space="preserve">R14 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14 needed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14 escalated to </t>
   </si>
   <si>
     <t xml:space="preserve">R14 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R14 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R14 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R14 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R15 name</t>
+    <t xml:space="preserve">R15 name </t>
   </si>
   <si>
     <t xml:space="preserve">R15 needed by</t>
@@ -631,10 +715,16 @@
     <t xml:space="preserve">R15 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R15 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R15 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R16 name</t>
+    <t xml:space="preserve">R16 name </t>
   </si>
   <si>
     <t xml:space="preserve">R16 needed by</t>
@@ -646,10 +736,16 @@
     <t xml:space="preserve">R16 type</t>
   </si>
   <si>
+    <t xml:space="preserve">R16 Central Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R16 Point of Contact</t>
+  </si>
+  <si>
     <t xml:space="preserve">R16 secured</t>
   </si>
   <si>
-    <t xml:space="preserve">R17 name</t>
+    <t xml:space="preserve">R17 name </t>
   </si>
   <si>
     <t xml:space="preserve">R17 needed by</t>
@@ -661,10 +757,7 @@
     <t xml:space="preserve">R17 type</t>
   </si>
   <si>
-    <t xml:space="preserve">R17 secured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18 name</t>
+    <t xml:space="preserve">R18 name </t>
   </si>
   <si>
     <t xml:space="preserve">R18 needed by</t>
@@ -676,10 +769,7 @@
     <t xml:space="preserve">R18 type</t>
   </si>
   <si>
-    <t xml:space="preserve">R18 secured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R19 name</t>
+    <t xml:space="preserve">R19 name </t>
   </si>
   <si>
     <t xml:space="preserve">R19 needed by</t>
@@ -691,10 +781,7 @@
     <t xml:space="preserve">R19 type</t>
   </si>
   <si>
-    <t xml:space="preserve">R19 secured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R20 name</t>
+    <t xml:space="preserve">R20 name </t>
   </si>
   <si>
     <t xml:space="preserve">R20 needed by</t>
@@ -704,9 +791,6 @@
   </si>
   <si>
     <t xml:space="preserve">R20 type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R20 secured</t>
   </si>
   <si>
     <t xml:space="preserve">PC1 name</t>
@@ -930,10 +1014,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U239"/>
+  <dimension ref="A1:U267"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2400,7 +2484,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="0" t="s">
         <v>129</v>
       </c>
       <c r="D108" s="1"/>
@@ -2415,7 +2499,7 @@
       <c r="U108" s="1"/>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="0" t="s">
         <v>130</v>
       </c>
       <c r="F109" s="2"/>
@@ -2429,17 +2513,17 @@
       <c r="U109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="0" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="0" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="0" t="s">
         <v>133</v>
       </c>
       <c r="F112" s="1"/>
@@ -2453,7 +2537,7 @@
       <c r="U112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="0" t="s">
         <v>134</v>
       </c>
       <c r="D113" s="1"/>
@@ -2465,7 +2549,7 @@
       <c r="U113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="0" t="s">
         <v>135</v>
       </c>
       <c r="D114" s="2"/>
@@ -2477,17 +2561,17 @@
       <c r="U114" s="2"/>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="s">
+      <c r="A115" s="0" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="s">
+      <c r="A116" s="0" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="s">
+      <c r="A117" s="0" t="s">
         <v>138</v>
       </c>
       <c r="F117" s="1"/>
@@ -2498,7 +2582,7 @@
       <c r="U117" s="1"/>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D118" s="1"/>
@@ -2509,7 +2593,7 @@
       <c r="U118" s="1"/>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="s">
+      <c r="A119" s="0" t="s">
         <v>140</v>
       </c>
       <c r="D119" s="2"/>
@@ -2520,17 +2604,17 @@
       <c r="U119" s="2"/>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="0" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="0" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="0" t="s">
         <v>143</v>
       </c>
       <c r="F122" s="1"/>
@@ -2540,7 +2624,7 @@
       <c r="U122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="0" t="s">
         <v>144</v>
       </c>
       <c r="D123" s="1"/>
@@ -2549,7 +2633,7 @@
       <c r="U123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="0" t="s">
         <v>145</v>
       </c>
       <c r="D124" s="2"/>
@@ -2558,17 +2642,17 @@
       <c r="U124" s="2"/>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="0" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="0" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="0" t="s">
         <v>148</v>
       </c>
       <c r="I127" s="1"/>
@@ -2576,407 +2660,407 @@
       <c r="U127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="s">
+      <c r="A128" s="0" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="s">
+      <c r="A129" s="0" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="0" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="s">
+      <c r="A131" s="0" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="s">
+      <c r="A132" s="0" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
+      <c r="A133" s="0" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="s">
+      <c r="A134" s="0" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
+      <c r="A135" s="0" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
+      <c r="A136" s="0" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
+      <c r="A137" s="0" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
+      <c r="A138" s="0" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
+      <c r="A139" s="0" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="0" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="0" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+      <c r="A142" s="0" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
+      <c r="A143" s="0" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
+      <c r="A144" s="0" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="s">
+      <c r="A145" s="0" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
+      <c r="A146" s="0" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="s">
+      <c r="A147" s="0" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="s">
+      <c r="A148" s="0" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="s">
+      <c r="A149" s="0" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
+      <c r="A150" s="0" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
+      <c r="A151" s="0" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="s">
+      <c r="A152" s="0" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="0" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="s">
+      <c r="A154" s="0" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="s">
+      <c r="A155" s="0" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
+      <c r="A156" s="0" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
+      <c r="A157" s="0" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
+      <c r="A158" s="0" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="s">
+      <c r="A159" s="0" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
+      <c r="A160" s="0" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
+      <c r="A161" s="0" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
+      <c r="A162" s="0" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="s">
+      <c r="A163" s="0" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
+      <c r="A164" s="0" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
+      <c r="A165" s="0" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
+      <c r="A166" s="0" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
+      <c r="A167" s="0" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
+      <c r="A168" s="0" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
+      <c r="A169" s="0" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
+      <c r="A170" s="0" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
+      <c r="A171" s="0" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="s">
+      <c r="A172" s="0" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="s">
+      <c r="A173" s="0" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="s">
+      <c r="A174" s="0" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
+      <c r="A175" s="0" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
+      <c r="A176" s="0" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
+      <c r="A177" s="0" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
+      <c r="A178" s="0" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
+      <c r="A179" s="0" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
+      <c r="A180" s="0" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
+      <c r="A181" s="0" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="s">
+      <c r="A182" s="0" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
+      <c r="A183" s="0" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
+      <c r="A184" s="0" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="s">
+      <c r="A185" s="0" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="1" t="s">
+      <c r="A186" s="0" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="s">
+      <c r="A187" s="0" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="s">
+      <c r="A188" s="0" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="1" t="s">
+      <c r="A189" s="0" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="s">
+      <c r="A190" s="0" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="1" t="s">
+      <c r="A191" s="0" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="1" t="s">
+      <c r="A192" s="0" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="s">
+      <c r="A193" s="0" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="s">
+      <c r="A194" s="0" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="1" t="s">
+      <c r="A195" s="0" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="1" t="s">
+      <c r="A196" s="0" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="s">
+      <c r="A197" s="0" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="s">
+      <c r="A198" s="0" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="1" t="s">
+      <c r="A199" s="0" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="s">
+      <c r="A200" s="0" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1" t="s">
+      <c r="A201" s="0" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
+      <c r="A202" s="0" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="s">
+      <c r="A203" s="0" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1" t="s">
+      <c r="A204" s="0" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="1" t="s">
+      <c r="A205" s="0" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1" t="s">
+      <c r="A206" s="0" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="s">
+      <c r="A207" s="0" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="s">
+      <c r="A208" s="0" t="s">
         <v>229</v>
       </c>
       <c r="C208" s="1"/>
@@ -2998,7 +3082,7 @@
       <c r="U208" s="1"/>
     </row>
     <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="1" t="s">
+      <c r="A209" s="0" t="s">
         <v>230</v>
       </c>
       <c r="C209" s="1"/>
@@ -3020,7 +3104,7 @@
       <c r="U209" s="1"/>
     </row>
     <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="1" t="s">
+      <c r="A210" s="0" t="s">
         <v>231</v>
       </c>
       <c r="C210" s="1"/>
@@ -3036,7 +3120,7 @@
       <c r="T210" s="1"/>
     </row>
     <row r="211" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1" t="s">
+      <c r="A211" s="0" t="s">
         <v>232</v>
       </c>
       <c r="C211" s="1"/>
@@ -3045,7 +3129,7 @@
       <c r="O211" s="1"/>
     </row>
     <row r="212" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A212" s="1" t="s">
+      <c r="A212" s="0" t="s">
         <v>233</v>
       </c>
       <c r="D212" s="1"/>
@@ -3064,7 +3148,7 @@
       <c r="U212" s="1"/>
     </row>
     <row r="213" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A213" s="1" t="s">
+      <c r="A213" s="0" t="s">
         <v>234</v>
       </c>
       <c r="D213" s="1"/>
@@ -3083,7 +3167,7 @@
       <c r="U213" s="1"/>
     </row>
     <row r="214" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A214" s="1" t="s">
+      <c r="A214" s="0" t="s">
         <v>235</v>
       </c>
       <c r="E214" s="1"/>
@@ -3097,13 +3181,13 @@
       <c r="T214" s="1"/>
     </row>
     <row r="215" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A215" s="1" t="s">
+      <c r="A215" s="0" t="s">
         <v>236</v>
       </c>
       <c r="K215" s="1"/>
     </row>
     <row r="216" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="s">
+      <c r="A216" s="0" t="s">
         <v>237</v>
       </c>
       <c r="H216" s="1"/>
@@ -3117,7 +3201,7 @@
       <c r="U216" s="1"/>
     </row>
     <row r="217" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A217" s="1" t="s">
+      <c r="A217" s="0" t="s">
         <v>238</v>
       </c>
       <c r="H217" s="1"/>
@@ -3131,7 +3215,7 @@
       <c r="U217" s="1"/>
     </row>
     <row r="218" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1" t="s">
+      <c r="A218" s="0" t="s">
         <v>239</v>
       </c>
       <c r="H218" s="1"/>
@@ -3142,14 +3226,14 @@
       <c r="T218" s="1"/>
     </row>
     <row r="219" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="1" t="s">
+      <c r="A219" s="0" t="s">
         <v>240</v>
       </c>
       <c r="K219" s="1"/>
       <c r="R219" s="1"/>
     </row>
     <row r="220" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A220" s="1" t="s">
+      <c r="A220" s="0" t="s">
         <v>241</v>
       </c>
       <c r="H220" s="1"/>
@@ -3161,7 +3245,7 @@
       <c r="U220" s="1"/>
     </row>
     <row r="221" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A221" s="1" t="s">
+      <c r="A221" s="0" t="s">
         <v>242</v>
       </c>
       <c r="H221" s="1"/>
@@ -3173,7 +3257,7 @@
       <c r="U221" s="1"/>
     </row>
     <row r="222" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A222" s="1" t="s">
+      <c r="A222" s="0" t="s">
         <v>243</v>
       </c>
       <c r="H222" s="1"/>
@@ -3183,94 +3267,234 @@
       <c r="T222" s="1"/>
     </row>
     <row r="223" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A223" s="1" t="s">
+      <c r="A223" s="0" t="s">
         <v>244</v>
       </c>
       <c r="R223" s="1"/>
     </row>
     <row r="224" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A224" s="1" t="s">
+      <c r="A224" s="0" t="s">
         <v>245</v>
       </c>
       <c r="H224" s="1"/>
       <c r="U224" s="1"/>
     </row>
     <row r="225" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A225" s="1" t="s">
+      <c r="A225" s="0" t="s">
         <v>246</v>
       </c>
       <c r="H225" s="1"/>
       <c r="U225" s="1"/>
     </row>
     <row r="226" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A226" s="1" t="s">
+      <c r="A226" s="0" t="s">
         <v>247</v>
       </c>
       <c r="H226" s="1"/>
     </row>
     <row r="227" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="1" t="s">
+      <c r="A227" s="0" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A228" s="1" t="s">
+      <c r="A228" s="0" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A229" s="1" t="s">
+      <c r="A229" s="0" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A230" s="1" t="s">
+      <c r="A230" s="0" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A231" s="1" t="s">
+      <c r="A231" s="0" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A232" s="1" t="s">
+      <c r="A232" s="0" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A233" s="1" t="s">
+      <c r="A233" s="0" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A234" s="1" t="s">
+      <c r="A234" s="0" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A235" s="1" t="s">
+      <c r="A235" s="0" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A236" s="1" t="s">
+      <c r="A236" s="0" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A237" s="1" t="s">
+      <c r="A237" s="0" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A238" s="1" t="s">
+      <c r="A238" s="0" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A239" s="1" t="s">
+      <c r="A239" s="0" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests update. all tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/250_master_test_1.xlsx
+++ b/tests/resources/250_master_test_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="369">
   <si>
     <t xml:space="preserve">PROJECT ID</t>
   </si>
@@ -409,6 +409,126 @@
     <t xml:space="preserve">MM20 Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">MM21 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM21 date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM21 status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM21 Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM22 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM22 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM22 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM22 Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM23 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM23 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM23 status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM23 Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM24 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM24 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM24 status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM24 Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM25 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM25 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM25 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM25 Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM26 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM26 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM26 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM26 Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM27 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM27 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM27 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM27 Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM28 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM28 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM28 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM28 Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM29 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM29 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM29 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM29 Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM30 name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM30 date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM30 status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM30 Comment</t>
+  </si>
+  <si>
     <t xml:space="preserve">R1 name </t>
   </si>
   <si>
@@ -791,6 +911,126 @@
   </si>
   <si>
     <t xml:space="preserve">R20 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29 type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30 name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30 needed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30 escalated to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30 type</t>
   </si>
   <si>
     <t xml:space="preserve">PC1 name</t>
@@ -1014,10 +1254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U267"/>
+  <dimension ref="A1:U347"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A309" activeCellId="0" sqref="A309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2484,7 +2724,7 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="1" t="s">
         <v>129</v>
       </c>
       <c r="D108" s="1"/>
@@ -2499,7 +2739,7 @@
       <c r="U108" s="1"/>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="1" t="s">
         <v>130</v>
       </c>
       <c r="F109" s="2"/>
@@ -2513,17 +2753,17 @@
       <c r="U109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="1" t="s">
         <v>133</v>
       </c>
       <c r="F112" s="1"/>
@@ -2537,7 +2777,7 @@
       <c r="U112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="A113" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D113" s="1"/>
@@ -2549,7 +2789,7 @@
       <c r="U113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="1" t="s">
         <v>135</v>
       </c>
       <c r="D114" s="2"/>
@@ -2561,17 +2801,17 @@
       <c r="U114" s="2"/>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="A115" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="A116" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="1" t="s">
         <v>138</v>
       </c>
       <c r="F117" s="1"/>
@@ -2582,7 +2822,7 @@
       <c r="U117" s="1"/>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="A118" s="1" t="s">
         <v>139</v>
       </c>
       <c r="D118" s="1"/>
@@ -2593,7 +2833,7 @@
       <c r="U118" s="1"/>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="A119" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D119" s="2"/>
@@ -2604,17 +2844,17 @@
       <c r="U119" s="2"/>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="A120" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="1" t="s">
         <v>143</v>
       </c>
       <c r="F122" s="1"/>
@@ -2624,7 +2864,7 @@
       <c r="U122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D123" s="1"/>
@@ -2633,7 +2873,7 @@
       <c r="U123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D124" s="2"/>
@@ -2642,17 +2882,17 @@
       <c r="U124" s="2"/>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="A125" s="1" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="A126" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+      <c r="A127" s="1" t="s">
         <v>148</v>
       </c>
       <c r="I127" s="1"/>
@@ -2660,102 +2900,102 @@
       <c r="U127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="A128" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+      <c r="A129" s="1" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="A130" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+      <c r="A131" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="A132" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+      <c r="A133" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+      <c r="A134" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+      <c r="A135" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="A136" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+      <c r="A137" s="1" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="A138" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="A139" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="A140" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+      <c r="A141" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="A142" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="A143" s="1" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
+      <c r="A144" s="1" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
+      <c r="A145" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="A146" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="A147" s="1" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3495,6 +3735,406 @@
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>